<commit_message>
added ui form and added validation function
</commit_message>
<xml_diff>
--- a/MCQ_OMR.xlsx
+++ b/MCQ_OMR.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8355" windowWidth="20385"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8355" windowWidth="20385"/>
   </bookViews>
   <sheets>
     <sheet name="answerkey" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="result" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
@@ -29,12 +30,125 @@
     <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="165"/>
     <numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="166"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -47,8 +161,16 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <color theme="1"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -60,134 +182,6 @@
       <u val="single"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -198,6 +192,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -210,13 +270,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,157 +342,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,6 +395,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -412,36 +421,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -462,6 +441,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -491,149 +485,149 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="164">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="165">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="166">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="8" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="12" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="6" numFmtId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="166">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="10" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="9" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="28" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="23" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="10" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="10" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="20" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="31" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="18" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="24" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="7" numFmtId="0">
+    <xf applyAlignment="1" borderId="7" fillId="31" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="27" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="15" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="26" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="15" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="24" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="19" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="18" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="22" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="21" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1367,8 +1361,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.142857142857141" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1393,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1432,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1732,6 +1726,42 @@
         <v>1</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.142857142857141" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7"/>
+    <row r="3" spans="1:7"/>
+    <row r="4" spans="1:7"/>
+    <row r="5" spans="1:7"/>
+    <row r="6" spans="1:7"/>
+    <row r="7" spans="1:7"/>
+    <row r="8" spans="1:7"/>
+    <row r="9" spans="1:7"/>
+    <row r="10" spans="1:7"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
result are compiled into sheet
</commit_message>
<xml_diff>
--- a/MCQ_OMR.xlsx
+++ b/MCQ_OMR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8355" windowWidth="20385"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8355" windowWidth="20385"/>
   </bookViews>
   <sheets>
     <sheet name="answerkey" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>Total :</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
   </si>
 </sst>
 </file>
@@ -41,6 +44,13 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="0"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -48,21 +58,7 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -83,6 +79,45 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <charset val="134"/>
       <b val="1"/>
       <color theme="3"/>
@@ -92,8 +127,38 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <b val="1"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -108,21 +173,6 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <b val="1"/>
       <color rgb="FFFA7D00"/>
       <sz val="11"/>
@@ -131,55 +181,8 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -192,6 +195,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -204,175 +279,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,8 +392,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -410,37 +446,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -460,33 +476,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="2" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="1" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
@@ -504,130 +507,130 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="10" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="9" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
+    <xf applyAlignment="1" borderId="4" fillId="8" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="13" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="22" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="18" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="21" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="26" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="26" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="31" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="24" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="19" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="2" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="28" fontId="2" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="31" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="15" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="15" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="4" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="24" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="23" fontId="1" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="27" fontId="1" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="14" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="18" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1361,7 +1364,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1737,32 +1740,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.142857142857141" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7"/>
-    <row r="3" spans="1:7"/>
-    <row r="4" spans="1:7"/>
-    <row r="5" spans="1:7"/>
-    <row r="6" spans="1:7"/>
-    <row r="7" spans="1:7"/>
-    <row r="8" spans="1:7"/>
-    <row r="9" spans="1:7"/>
-    <row r="10" spans="1:7"/>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>